<commit_message>
added cleaning whitespaces for country column
</commit_message>
<xml_diff>
--- a/top_10_countries_raw_num.xlsx
+++ b/top_10_countries_raw_num.xlsx
@@ -449,33 +449,33 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> United Kingdom</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>60</v>
       </c>
       <c r="C2" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Greece</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>18</v>
       </c>
       <c r="C3" t="n">
-        <v>730</v>
+        <v>734</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> United States</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -488,7 +488,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> France</t>
+          <t>France</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -501,7 +501,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Italy</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -514,66 +514,66 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Poland</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>90</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Norway</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>176</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Romania</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>70</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iceland</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>23</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Japan</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>7</v>
       </c>
       <c r="C11" t="n">
-        <v>302</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>